<commit_message>
updated test file names
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/dua_one.xlsx
+++ b/tests/testthat/testdata/dua_one.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bts4h/packages/duawranglr/tests/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bts4h/packages/duawranglr/tests/testthat/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FFC2568-E28C-C947-8AD1-4F344F2DA498}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{59897225-4D10-6549-B751-B8533AA9EABC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>level_i</t>
   </si>
@@ -31,31 +31,28 @@
     <t>level_iii</t>
   </si>
   <si>
-    <t>student_id</t>
-  </si>
-  <si>
-    <t>name</t>
+    <t>sid</t>
+  </si>
+  <si>
+    <t>sname</t>
   </si>
   <si>
     <t>dob</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
-    <t>zip_code</t>
-  </si>
-  <si>
     <t>raceeth</t>
   </si>
   <si>
-    <t>teacher_id</t>
-  </si>
-  <si>
-    <t>teacher_name</t>
+    <t>tid</t>
+  </si>
+  <si>
+    <t>tname</t>
+  </si>
+  <si>
+    <t>zip</t>
   </si>
 </sst>
 </file>
@@ -942,63 +939,39 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>